<commit_message>
NCB-530 still not test
</commit_message>
<xml_diff>
--- a/inputdata/NCB_530.xlsx
+++ b/inputdata/NCB_530.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="NCB_530" sheetId="18" r:id="rId1"/>
-    <sheet name="Name" sheetId="30" r:id="rId2"/>
+    <sheet name="NAME" sheetId="30" r:id="rId2"/>
     <sheet name="PAYMENT_METHOD" sheetId="19" r:id="rId3"/>
     <sheet name="PAYMENT_CHANNEL" sheetId="20" r:id="rId4"/>
     <sheet name="VIRTUAL" sheetId="21" r:id="rId5"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="111">
   <si>
     <t>ID</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>GROUP_Praxis</t>
+  </si>
+  <si>
+    <t>PC_1/PC_2/PC_3/PC_4/PC_5</t>
   </si>
 </sst>
 </file>
@@ -764,7 +767,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -773,7 +776,7 @@
     <col min="2" max="2" width="21.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
@@ -844,7 +847,7 @@
         <v>54</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>65</v>
@@ -888,7 +891,7 @@
         <v>55</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>65</v>
@@ -932,7 +935,7 @@
         <v>56</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>65</v>
@@ -1286,7 +1289,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,7 +1384,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,7 +1551,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>